<commit_message>
Se crear el archivo readme
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/DatoDePrueba.xlsx
+++ b/src/test/resources/Data/DatoDePrueba.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanbumn\Documents\Repositorios\CapacitacionQvision\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03095DD-BCFA-4D20-877C-30EFA5378C5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAF95BA-F900-4949-BE5E-F85E2121D009}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,7 +372,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se actualiza el build.gradle
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/DatoDePrueba.xlsx
+++ b/src/test/resources/Data/DatoDePrueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanbumn\Documents\Repositorios\CapacitacionQvision\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAF95BA-F900-4949-BE5E-F85E2121D009}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42799D85-00D7-4E13-967D-C149F7EE70DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>pistola</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>maria</t>
+  </si>
+  <si>
+    <t>maria@reqres.in</t>
   </si>
 </sst>
 </file>
@@ -369,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,6 +408,14 @@
       </c>
       <c r="C3" s="1"/>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se suben las ajustes de las pruebas al servicio
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/DatoDePrueba.xlsx
+++ b/src/test/resources/Data/DatoDePrueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanbumn\Documents\Repositorios\CapacitacionQvision\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42799D85-00D7-4E13-967D-C149F7EE70DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095AF86C-7C8C-4421-8D79-B07386A70350}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -375,7 +375,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>